<commit_message>
Add Excel backup and restore files, update templates
Added backup and restored versions of multiple PO Excel files under new directories. Updated several existing Excel and JSON template files for order generation, and added new product and color images. Also included scripts for restoring Excel formatting.
</commit_message>
<xml_diff>
--- a/order_generation/PO_excel_selected/17-A1KN-KJGW.xlsx
+++ b/order_generation/PO_excel_selected/17-A1KN-KJGW.xlsx
@@ -15,9 +15,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0&quot;PCS&quot;"/>
     <numFmt numFmtId="165" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -256,7 +257,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -421,6 +422,9 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -522,7 +526,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
         <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
@@ -569,7 +573,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="email" r:embed="rId5"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="email" r:embed="rId6"/>
         <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
@@ -616,7 +620,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="email" r:embed="rId6"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="email" r:embed="rId7"/>
         <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
@@ -663,7 +667,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
         <a:srcRect xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
@@ -710,7 +714,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -751,7 +755,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -792,7 +796,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -833,7 +837,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -874,7 +878,7 @@
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1016,13 +1020,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId13"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1380,7 +1387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
@@ -1544,8 +1551,8 @@
           <t>白色针+黑色（TPR）胶皮参考denman样品，手柄571U透明弹性漆，背面印白色logo 包装方式：纸卡包装系扎带，包装背面贴fba不干胶，套opp袋，注意单箱不要超过100个</t>
         </is>
       </c>
-      <c r="D7" s="59" t="n">
-        <v>0</v>
+      <c r="D7" s="61" t="n">
+        <v>25569.33333333333</v>
       </c>
       <c r="E7" s="60" t="n">
         <v>5.14</v>
@@ -1864,16 +1871,9 @@
     <row r="34" ht="21" customFormat="1" customHeight="1" s="6">
       <c r="H34" s="15" t="n"/>
     </row>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
     <row r="38">
       <c r="H38" s="15" t="n"/>
     </row>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="11" t="n"/>
       <c r="B43" s="13" t="n"/>
@@ -1974,7 +1974,6 @@
       <c r="A67" s="11" t="n"/>
       <c r="B67" s="13" t="n"/>
     </row>
-    <row r="68"/>
     <row r="69" ht="17.25" customHeight="1">
       <c r="B69" s="9" t="inlineStr">
         <is>
@@ -2006,42 +2005,25 @@
       </c>
       <c r="F70" s="14" t="n"/>
     </row>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
     <row r="80">
       <c r="H80" s="15" t="n"/>
     </row>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.393700787401575" right="0.393700787401575" top="0.78740157480315" bottom="0.590551181102362" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>